<commit_message>
adding new data and putting "-" in place of 0
</commit_message>
<xml_diff>
--- a/private/values/newFile.xlsx
+++ b/private/values/newFile.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,466 +416,721 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Beans</v>
+        <v>Apple</v>
       </c>
       <c r="B3" t="str">
-        <v>3.71</v>
+        <v>0.29</v>
       </c>
       <c r="C3" t="str">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="D3" t="str">
-        <v>2.85</v>
+        <v>13.11</v>
       </c>
       <c r="E3" t="str">
-        <v>33.46</v>
+        <v>62.64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Butter</v>
+        <v>Beans</v>
       </c>
       <c r="B4" t="str">
-        <v>0.85</v>
+        <v>3.71</v>
       </c>
       <c r="C4" t="str">
-        <v>81.11</v>
+        <v>0.6</v>
       </c>
       <c r="D4" t="str">
-        <v>0.06</v>
+        <v>2.85</v>
       </c>
       <c r="E4" t="str">
-        <v>717</v>
+        <v>33.46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Capsicum</v>
+        <v>Butter</v>
       </c>
       <c r="B5" t="str">
-        <v>1.11</v>
+        <v>0.85</v>
       </c>
       <c r="C5" t="str">
-        <v>0.34</v>
+        <v>81.11</v>
       </c>
       <c r="D5" t="str">
-        <v>1.84</v>
+        <v>0.06</v>
       </c>
       <c r="E5" t="str">
-        <v>16.25</v>
+        <v>717</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Carrot</v>
+        <v>Capsicum</v>
       </c>
       <c r="B6" t="str">
-        <v>1.04</v>
+        <v>1.11</v>
       </c>
       <c r="C6" t="str">
-        <v>0.47</v>
+        <v>0.34</v>
       </c>
       <c r="D6" t="str">
-        <v>6.71</v>
+        <v>1.84</v>
       </c>
       <c r="E6" t="str">
-        <v>38.24</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Chicken</v>
+        <v>Carrot</v>
       </c>
       <c r="B7" t="str">
-        <v>21.81</v>
+        <v>1.04</v>
       </c>
       <c r="C7" t="str">
-        <v>9</v>
+        <v>0.47</v>
       </c>
       <c r="D7" t="str">
-        <v>0</v>
+        <v>6.71</v>
       </c>
       <c r="E7" t="str">
-        <v>168.26</v>
+        <v>38.24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Curd</v>
+        <v>Chicken</v>
       </c>
       <c r="B8" t="str">
-        <v>3.1</v>
+        <v>21.81</v>
       </c>
       <c r="C8" t="str">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D8" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" t="str">
-        <v>60</v>
+        <v>168.26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Custard Powder</v>
+        <v>Coriander</v>
       </c>
       <c r="B9" t="str">
-        <v>1.9</v>
+        <v>3.52</v>
       </c>
       <c r="C9" t="str">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="D9" t="str">
-        <v>84</v>
+        <v>1.93</v>
       </c>
       <c r="E9" t="str">
-        <v>357</v>
+        <v>31.07</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Dalia</v>
+        <v>Corn</v>
       </c>
       <c r="B10" t="str">
-        <v>10.84</v>
+        <v>2.69</v>
       </c>
       <c r="C10" t="str">
-        <v>1.45</v>
+        <v>1.33</v>
       </c>
       <c r="D10" t="str">
-        <v>69.06</v>
+        <v>11.66</v>
       </c>
       <c r="E10" t="str">
-        <v>341.78</v>
+        <v>73.14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Egg (boiled)</v>
+        <v>Corn flour</v>
       </c>
       <c r="B11" t="str">
-        <v>12.37</v>
+        <v>1.2</v>
       </c>
       <c r="C11" t="str">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="D11" t="str">
-        <v>0</v>
+        <v>88.4</v>
       </c>
       <c r="E11" t="str">
-        <v>52.58</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Egg (raw)</v>
+        <v>Cucumber</v>
       </c>
       <c r="B12" t="str">
-        <v>10.84</v>
+        <v>0.71</v>
       </c>
       <c r="C12" t="str">
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="D12" t="str">
-        <v>0</v>
+        <v>3.48</v>
       </c>
       <c r="E12" t="str">
-        <v>44.69</v>
+        <v>19.6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Gourd</v>
+        <v>Curd</v>
       </c>
       <c r="B13" t="str">
-        <v>0.49</v>
+        <v>3.1</v>
       </c>
       <c r="C13" t="str">
-        <v>0.13</v>
+        <v>4</v>
       </c>
       <c r="D13" t="str">
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="E13" t="str">
-        <v>12.91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Lentil</v>
+        <v>Custard Powder</v>
       </c>
       <c r="B14" t="str">
-        <v>22.87</v>
+        <v>1.9</v>
       </c>
       <c r="C14" t="str">
-        <v>0.61</v>
+        <v>1.5</v>
       </c>
       <c r="D14" t="str">
-        <v>47.91</v>
+        <v>84</v>
       </c>
       <c r="E14" t="str">
-        <v>297.8</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Lettuce</v>
+        <v>Dalia</v>
       </c>
       <c r="B15" t="str">
-        <v>1.54</v>
+        <v>10.84</v>
       </c>
       <c r="C15" t="str">
-        <v>0.27</v>
+        <v>1.45</v>
       </c>
       <c r="D15" t="str">
-        <v>3.01</v>
+        <v>69.06</v>
       </c>
       <c r="E15" t="str">
-        <v>21.75</v>
+        <v>341.78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Mango</v>
+        <v>Egg (boiled)</v>
       </c>
       <c r="B16" t="str">
-        <v>0.46</v>
+        <v>12.37</v>
       </c>
       <c r="C16" t="str">
-        <v>0.54</v>
+        <v>0.26</v>
       </c>
       <c r="D16" t="str">
-        <v>9.03</v>
+        <v>0</v>
       </c>
       <c r="E16" t="str">
-        <v>44.69</v>
+        <v>52.58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Milk</v>
+        <v>Egg (raw)</v>
       </c>
       <c r="B17" t="str">
-        <v>3.26</v>
+        <v>10.84</v>
       </c>
       <c r="C17" t="str">
-        <v>4.48</v>
+        <v>0.06</v>
       </c>
       <c r="D17" t="str">
-        <v>4.94</v>
+        <v>0</v>
       </c>
       <c r="E17" t="str">
-        <v>72.9</v>
+        <v>44.69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Oil</v>
+        <v>Gourd</v>
       </c>
       <c r="B18" t="str">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="C18" t="str">
-        <v>100</v>
+        <v>0.13</v>
       </c>
       <c r="D18" t="str">
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="E18" t="str">
-        <v>900</v>
+        <v>12.91</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Onion</v>
+        <v>Guava</v>
       </c>
       <c r="B19" t="str">
-        <v>1.5</v>
+        <v>1.44</v>
       </c>
       <c r="C19" t="str">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="D19" t="str">
-        <v>9.56</v>
+        <v>5.13</v>
       </c>
       <c r="E19" t="str">
-        <v>48.04</v>
+        <v>32.27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Peas</v>
+        <v>Lentil</v>
       </c>
       <c r="B20" t="str">
-        <v>7.25</v>
+        <v>22.87</v>
       </c>
       <c r="C20" t="str">
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="D20" t="str">
-        <v>11.88</v>
+        <v>47.91</v>
       </c>
       <c r="E20" t="str">
-        <v>81.26</v>
+        <v>297.8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Pineapple</v>
+        <v>Lettuce</v>
       </c>
       <c r="B21" t="str">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="C21" t="str">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="D21" t="str">
-        <v>9.42</v>
+        <v>3.01</v>
       </c>
       <c r="E21" t="str">
-        <v>43.02</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Potato</v>
+        <v>Mango</v>
       </c>
       <c r="B22" t="str">
-        <v>1.54</v>
+        <v>0.46</v>
       </c>
       <c r="C22" t="str">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="D22" t="str">
-        <v>14.89</v>
+        <v>9.03</v>
       </c>
       <c r="E22" t="str">
-        <v>69.79</v>
+        <v>44.69</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Rice</v>
+        <v>Milk</v>
       </c>
       <c r="B23" t="str">
-        <v>7.94</v>
+        <v>3.26</v>
       </c>
       <c r="C23" t="str">
-        <v>0.52</v>
+        <v>4.48</v>
       </c>
       <c r="D23" t="str">
-        <v>78.24</v>
+        <v>4.94</v>
       </c>
       <c r="E23" t="str">
-        <v>356.36</v>
+        <v>72.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Semolina</v>
+        <v>Oats</v>
       </c>
       <c r="B24" t="str">
-        <v>11.38</v>
+        <v>13.6</v>
       </c>
       <c r="C24" t="str">
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="D24" t="str">
-        <v>68.43</v>
+        <v>62.8</v>
       </c>
       <c r="E24" t="str">
-        <v>333.65</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Skimmed Milk</v>
+        <v>Oil</v>
       </c>
       <c r="B25" t="str">
-        <v>3.37</v>
+        <v>0</v>
       </c>
       <c r="C25" t="str">
-        <v>0.08</v>
+        <v>100</v>
       </c>
       <c r="D25" t="str">
-        <v>4.89</v>
+        <v>0</v>
       </c>
       <c r="E25" t="str">
-        <v>34</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Spinach</v>
+        <v>Onion</v>
       </c>
       <c r="B26" t="str">
-        <v>2.14</v>
+        <v>1.5</v>
       </c>
       <c r="C26" t="str">
-        <v>0.64</v>
+        <v>0</v>
       </c>
       <c r="D26" t="str">
-        <v>2.05</v>
+        <v>9.56</v>
       </c>
       <c r="E26" t="str">
-        <v>24.38</v>
+        <v>48.04</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Tomato</v>
+        <v>Paneer</v>
       </c>
       <c r="B27" t="str">
-        <v>0.9</v>
+        <v>18.86</v>
       </c>
       <c r="C27" t="str">
-        <v>0.47</v>
+        <v>14.78</v>
       </c>
       <c r="D27" t="str">
-        <v>2.71</v>
+        <v>12.41</v>
       </c>
       <c r="E27" t="str">
-        <v>19.6</v>
+        <v>257.89</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Vermicelli</v>
+        <v>Papaya (raw)</v>
       </c>
       <c r="B28" t="str">
-        <v>9.7</v>
+        <v>0.5</v>
       </c>
       <c r="C28" t="str">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="D28" t="str">
-        <v>70.39</v>
+        <v>4.4</v>
       </c>
       <c r="E28" t="str">
-        <v>332.7</v>
+        <v>23.92</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
+        <v>Papaya (ripe)</v>
+      </c>
+      <c r="B29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C29" t="str">
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <v>4.61</v>
+      </c>
+      <c r="E29" t="str">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Pear</v>
+      </c>
+      <c r="B30" t="str">
+        <v>0</v>
+      </c>
+      <c r="C30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D30" t="str">
+        <v>8.09</v>
+      </c>
+      <c r="E30" t="str">
+        <v>37.52</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Peas</v>
+      </c>
+      <c r="B31" t="str">
+        <v>7.25</v>
+      </c>
+      <c r="C31" t="str">
+        <v>0</v>
+      </c>
+      <c r="D31" t="str">
+        <v>11.88</v>
+      </c>
+      <c r="E31" t="str">
+        <v>81.26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Pineapple</v>
+      </c>
+      <c r="B32" t="str">
+        <v>0</v>
+      </c>
+      <c r="C32" t="str">
+        <v>0</v>
+      </c>
+      <c r="D32" t="str">
+        <v>9.42</v>
+      </c>
+      <c r="E32" t="str">
+        <v>43.02</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Potato</v>
+      </c>
+      <c r="B33" t="str">
+        <v>1.54</v>
+      </c>
+      <c r="C33" t="str">
+        <v>0</v>
+      </c>
+      <c r="D33" t="str">
+        <v>14.89</v>
+      </c>
+      <c r="E33" t="str">
+        <v>69.79</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Puffed rice</v>
+      </c>
+      <c r="B34" t="str">
+        <v>7.47</v>
+      </c>
+      <c r="C34" t="str">
+        <v>1.62</v>
+      </c>
+      <c r="D34" t="str">
+        <v>77.68</v>
+      </c>
+      <c r="E34" t="str">
+        <v>361.85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Rice</v>
+      </c>
+      <c r="B35" t="str">
+        <v>7.94</v>
+      </c>
+      <c r="C35" t="str">
+        <v>0.52</v>
+      </c>
+      <c r="D35" t="str">
+        <v>78.24</v>
+      </c>
+      <c r="E35" t="str">
+        <v>356.36</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Rice flakes</v>
+      </c>
+      <c r="B36" t="str">
+        <v>7.44</v>
+      </c>
+      <c r="C36" t="str">
+        <v>1.14</v>
+      </c>
+      <c r="D36" t="str">
+        <v>76.75</v>
+      </c>
+      <c r="E36" t="str">
+        <v>353.73</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Semolina</v>
+      </c>
+      <c r="B37" t="str">
+        <v>11.38</v>
+      </c>
+      <c r="C37" t="str">
+        <v>0</v>
+      </c>
+      <c r="D37" t="str">
+        <v>68.43</v>
+      </c>
+      <c r="E37" t="str">
+        <v>333.65</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Skimmed Milk</v>
+      </c>
+      <c r="B38" t="str">
+        <v>3.37</v>
+      </c>
+      <c r="C38" t="str">
+        <v>0.08</v>
+      </c>
+      <c r="D38" t="str">
+        <v>4.89</v>
+      </c>
+      <c r="E38" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Spinach</v>
+      </c>
+      <c r="B39" t="str">
+        <v>2.14</v>
+      </c>
+      <c r="C39" t="str">
+        <v>0.64</v>
+      </c>
+      <c r="D39" t="str">
+        <v>2.05</v>
+      </c>
+      <c r="E39" t="str">
+        <v>24.38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Sugar</v>
+      </c>
+      <c r="B40" t="str">
+        <v>0.1</v>
+      </c>
+      <c r="C40" t="str">
+        <v>0</v>
+      </c>
+      <c r="D40" t="str">
+        <v>99.4</v>
+      </c>
+      <c r="E40" t="str">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Sweet potato</v>
+      </c>
+      <c r="B41" t="str">
+        <v>1.27</v>
+      </c>
+      <c r="C41" t="str">
+        <v>0</v>
+      </c>
+      <c r="D41" t="str">
+        <v>23.93</v>
+      </c>
+      <c r="E41" t="str">
+        <v>108.03</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Tomato</v>
+      </c>
+      <c r="B42" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="C42" t="str">
+        <v>0.47</v>
+      </c>
+      <c r="D42" t="str">
+        <v>2.71</v>
+      </c>
+      <c r="E42" t="str">
+        <v>19.6</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vermicelli</v>
+      </c>
+      <c r="B43" t="str">
+        <v>9.7</v>
+      </c>
+      <c r="C43" t="str">
+        <v>0</v>
+      </c>
+      <c r="D43" t="str">
+        <v>70.39</v>
+      </c>
+      <c r="E43" t="str">
+        <v>332.7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
         <v>Wheat flour</v>
       </c>
-      <c r="B29" t="str">
+      <c r="B44" t="str">
         <v>29.2</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C44" t="str">
         <v>7.4</v>
       </c>
-      <c r="D29" t="str">
+      <c r="D44" t="str">
         <v>53.3</v>
       </c>
-      <c r="E29" t="str">
+      <c r="E44" t="str">
         <v>397</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>